<commit_message>
Stage 1 Tasks A1-A6
</commit_message>
<xml_diff>
--- a/ptts55/evidence.xlsx
+++ b/ptts55/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -100,34 +100,58 @@
     <t xml:space="preserve">ClassID</t>
   </si>
   <si>
-    <t xml:space="preserve">tx hash on irisnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class id you issued</t>
+    <t xml:space="preserve">DBFA84F1F3BC67E079F5DC4EA71D5AEC71DBC6F05B1FD50A813C06E329DA362C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tstvchNFT</t>
   </si>
   <si>
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
-    <t xml:space="preserve">nft id you minted</t>
+    <t xml:space="preserve">A1BA957D83F70D373223AFE68617A349355D24F943C4211AE6F79C5E97B9313A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testovichNFT001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1B2B78F5C56A7B2CDC30F7622CEB0F9C0B4D517A69E018BE0A6CF2A3E78113DF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testovichNFT002</t>
   </si>
   <si>
     <t xml:space="preserve">ChainID</t>
   </si>
   <si>
-    <t xml:space="preserve">ibc class on dest chain</t>
+    <t xml:space="preserve">2B465AED8EFE538116368D2F9497D7319A26F1CE310AFFF1BEEDA7240D162D63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stars1gcaetd6459xscezwrnjvwn37tladk4jx42396ggnfz3a2743l2as6n8j8t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elgafar-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A979C7DD86F3C1FD4EB67CC1E6E8ACBFFDFFB17D767CEA88C6091F5AE528CE2C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/63D1D3D2925DEBF6AA6C8356880EF4518801A96CE2E2C556C24ED36FA9B7F5B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uptick_7000-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07B790D0BD13DBF2D896C18A1D1836049AC8DE1020D5A7165EA03D1D31DDEDD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">519C01F43D751379804DC024ECE8555EBB87DCB13C6CDE943C4E2BD29CB6C201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">nft id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest chain id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on dest chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -152,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -181,6 +205,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -252,7 +289,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,6 +311,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,11 +401,11 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.86"/>
@@ -446,7 +491,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -462,10 +507,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -490,7 +535,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -506,10 +551,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -534,7 +579,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -550,10 +595,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -574,11 +619,11 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -594,10 +639,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -622,7 +667,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -633,25 +678,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -676,7 +721,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -687,25 +732,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -730,7 +775,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -741,25 +786,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -784,7 +829,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -795,25 +840,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -838,7 +883,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -849,25 +894,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -892,7 +937,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -903,25 +948,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -946,7 +991,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
   </cols>
@@ -989,7 +1034,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -1000,25 +1045,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1043,7 +1088,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -1054,25 +1099,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1097,7 +1142,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
   </cols>
@@ -1109,12 +1154,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1139,7 +1184,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
   </cols>
@@ -1151,12 +1196,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1181,7 +1226,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
   </cols>
@@ -1193,12 +1238,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1268,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
   </cols>
@@ -1235,12 +1280,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1259,13 +1304,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
@@ -1284,13 +1329,24 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1371,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
@@ -1333,21 +1389,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1372,7 +1428,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
@@ -1390,21 +1446,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +1485,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
@@ -1447,21 +1503,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1486,7 +1542,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16"/>
@@ -1505,21 +1561,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1544,7 +1600,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -1560,10 +1616,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1588,7 +1644,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.43"/>
@@ -1604,10 +1660,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix A4 A6; Add B1 B2
</commit_message>
<xml_diff>
--- a/ptts55/evidence.xlsx
+++ b/ptts55/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">ibc/63D1D3D2925DEBF6AA6C8356880EF4518801A96CE2E2C556C24ED36FA9B7F5B1</t>
   </si>
   <si>
-    <t xml:space="preserve">Uptick_7000-2</t>
+    <t xml:space="preserve">uptick_7000-2</t>
   </si>
   <si>
     <t xml:space="preserve">07B790D0BD13DBF2D896C18A1D1836049AC8DE1020D5A7165EA03D1D31DDEDD0</t>
@@ -196,9 +196,6 @@
     <t xml:space="preserve">CF19B985A00D19B024467A7EF12666066B630563C46A4344DFC52519C9CBB533</t>
   </si>
   <si>
-    <t xml:space="preserve">uptick_7000-2</t>
-  </si>
-  <si>
     <t xml:space="preserve">2554D59305845D46C67667EA254DF7FD9A162BA70007AAF5440470F00AAD18B6</t>
   </si>
   <si>
@@ -302,6 +299,18 @@
   </si>
   <si>
     <t xml:space="preserve">C8D67AC553F949F22B637F7AD798EC7E540DAF5EDF77D106DD4D5E70B681EA1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F705B0C56E3ED3F5AB6F948C0E682EA2B8567D3BE3A46082C743B616E74AD286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E7B6B928963AA3FD27522852DE0F7812D211837DD7CEA9D3DFD7A212E150D678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B126D40FA0DE01443BD35F9B417BFFC8AE817BAC16315650063A56CC4F931A88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">721E3218B7D72A06E21BFC9210DA9A750B29DCF7D27A657ABBAB962F34593225</t>
   </si>
   <si>
     <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
@@ -852,12 +861,12 @@
         <v>49</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>28</v>
@@ -901,7 +910,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
@@ -909,26 +918,26 @@
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -969,7 +978,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
@@ -977,26 +986,26 @@
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1046,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
@@ -1045,15 +1054,15 @@
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>28</v>
@@ -1061,10 +1070,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1114,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
@@ -1113,7 +1122,7 @@
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>28</v>
@@ -1121,15 +1130,15 @@
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>28</v>
@@ -1173,7 +1182,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
@@ -1181,26 +1190,26 @@
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1284,7 +1293,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
@@ -1292,7 +1301,7 @@
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>28</v>
@@ -1300,31 +1309,31 @@
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>28</v>
@@ -1348,7 +1357,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1368,7 +1377,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
@@ -1376,15 +1385,15 @@
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>28</v>
@@ -1392,15 +1401,15 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>28</v>
@@ -1408,94 +1417,94 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1532,12 +1541,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1574,12 +1583,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>